<commit_message>
Updated Results for part one
</commit_message>
<xml_diff>
--- a/data/PartOne/Results/CrossValidation.xlsx
+++ b/data/PartOne/Results/CrossValidation.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Centered" sheetId="3" r:id="rId2"/>
+    <sheet name="Centered" sheetId="5" r:id="rId2"/>
     <sheet name="Standardized" sheetId="2" r:id="rId3"/>
     <sheet name="Whitened" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
   <si>
     <t>lambda</t>
   </si>
@@ -36,34 +36,7 @@
     <t>Mean Squares</t>
   </si>
   <si>
-    <t>Gradient Descent</t>
-  </si>
-  <si>
     <t>learning rate</t>
-  </si>
-  <si>
-    <t>1 e-6</t>
-  </si>
-  <si>
-    <t>1 e-9</t>
-  </si>
-  <si>
-    <t>1 e-12</t>
-  </si>
-  <si>
-    <t>1 e-13</t>
-  </si>
-  <si>
-    <t>1 e-11</t>
-  </si>
-  <si>
-    <t>0.5 e-12</t>
-  </si>
-  <si>
-    <t>0.25 e-12</t>
-  </si>
-  <si>
-    <t>0.75 e-12</t>
   </si>
   <si>
     <t>Gradient Descent Standardized lr = 0.1</t>
@@ -123,7 +96,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,8 +168,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,8 +210,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -256,6 +250,15 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -291,6 +294,15 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="A1:C23"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -636,20 +648,18 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="8"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="7"/>
+      <c r="J1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -661,15 +671,12 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
@@ -690,15 +697,9 @@
       <c r="C3" s="4">
         <v>3101.17</v>
       </c>
-      <c r="E3" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3.71964293234466E+16</v>
-      </c>
-      <c r="G3" s="4">
-        <v>3.7172049799606496E+16</v>
-      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="I3" s="4">
         <v>0</v>
       </c>
@@ -719,15 +720,9 @@
       <c r="C4" s="4">
         <v>3104.64</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4">
-        <v>378301453756.89001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>378104442775.37598</v>
-      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="I4" s="4">
         <v>0.01</v>
       </c>
@@ -748,15 +743,9 @@
       <c r="C5" s="4">
         <v>3105.54</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4">
-        <v>292864381.22248203</v>
-      </c>
-      <c r="G5" s="4">
-        <v>292864381.22248203</v>
-      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="I5" s="4">
         <v>0.05</v>
       </c>
@@ -773,15 +762,9 @@
       <c r="C6" s="4">
         <v>3096.1860000000001</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2650286.1090922002</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2654787.8196889702</v>
-      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="I6" s="4">
         <v>0.1</v>
       </c>
@@ -802,15 +785,9 @@
       <c r="C7" s="4">
         <v>3091.94</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4">
-        <v>19186.708374939401</v>
-      </c>
-      <c r="G7" s="4">
-        <v>19306.554436987099</v>
-      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="I7" s="4">
         <v>0.5</v>
       </c>
@@ -827,15 +804,7 @@
       <c r="C8" s="4">
         <v>3097.37</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>15372.1698716912</v>
-      </c>
-      <c r="G8">
-        <v>15375.7646003767</v>
-      </c>
+      <c r="E8" s="6"/>
       <c r="I8" s="4">
         <v>1</v>
       </c>
@@ -856,15 +825,9 @@
       <c r="C9" s="4">
         <v>3077.7489999999998</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4">
-        <v>11771.460691259501</v>
-      </c>
-      <c r="G9" s="4">
-        <v>11711.375691938299</v>
-      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="I9" s="4">
         <v>5</v>
       </c>
@@ -881,15 +844,7 @@
       <c r="C10" s="4">
         <v>3075.1959999999999</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10">
-        <v>23653.529710582399</v>
-      </c>
-      <c r="G10">
-        <v>23600.8839922316</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="I10" s="4">
         <v>10</v>
       </c>
@@ -910,15 +865,9 @@
       <c r="C11" s="4">
         <v>3062.663</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4">
-        <v>15916.338387661201</v>
-      </c>
-      <c r="G11" s="4">
-        <v>16005.675414555801</v>
-      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="I11" s="4">
         <v>2000</v>
       </c>
@@ -939,9 +888,7 @@
       <c r="C12" s="4">
         <v>3056.9459999999999</v>
       </c>
-      <c r="E12" s="6">
-        <v>5.0000000000000002E-5</v>
-      </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="I12" s="4">
@@ -964,9 +911,7 @@
       <c r="C13" s="4">
         <v>3041.0819999999999</v>
       </c>
-      <c r="E13" s="6">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="I13" s="4">
@@ -1035,6 +980,9 @@
       <c r="C16" s="4">
         <v>3033.4401349672598</v>
       </c>
+      <c r="D16" s="4">
+        <v>3129.5198733453499</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1201,7 +1149,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="I25" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>1</v>
@@ -1416,261 +1364,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>0</v>
       </c>
       <c r="B3" s="4">
-        <v>3025.21</v>
+        <v>3030.8838000587898</v>
       </c>
       <c r="C3" s="4">
-        <v>3101.17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>3090.1830680592002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>3025.51</v>
+        <v>3025.5882940432102</v>
       </c>
       <c r="C4" s="4">
-        <v>3104.64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>3080.7091797644898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
-        <v>0.05</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
-        <v>3025.52</v>
+        <v>3022.66262444621</v>
       </c>
       <c r="C5" s="4">
-        <v>3105.54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>3068.8713765102002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
-        <v>0.1</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4">
-        <v>3025.36</v>
+        <v>3013.5348438385099</v>
       </c>
       <c r="C6" s="4">
-        <v>3096.1860000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>3047.8725697555201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="4">
-        <v>3025.069</v>
+        <v>2956.90168127887</v>
       </c>
       <c r="C7" s="4">
-        <v>3091.94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2965.7838555051499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="B8" s="4">
-        <v>3024.8969999999999</v>
+        <v>2902.7234398262899</v>
       </c>
       <c r="C8" s="4">
-        <v>3097.37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>2906.7193416670402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
-        <v>5</v>
+        <v>3000</v>
       </c>
       <c r="B9" s="4">
-        <v>3023.84</v>
+        <v>2855.6467526349702</v>
       </c>
       <c r="C9" s="4">
-        <v>3077.7489999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2861.0411966847801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
-        <v>10</v>
+        <v>5000</v>
       </c>
       <c r="B10" s="4">
-        <v>3023.2159999999999</v>
+        <v>2780.7021264375799</v>
       </c>
       <c r="C10" s="4">
-        <v>3075.1959999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>2786.9019318906599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
-        <v>50</v>
+        <v>9000</v>
       </c>
       <c r="B11" s="4">
-        <v>3021.1379999999999</v>
+        <v>2691.3691210522602</v>
       </c>
       <c r="C11" s="4">
-        <v>3062.663</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>2697.8909048887999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="B12" s="4">
-        <v>3020.2489999999998</v>
+        <v>2678.6793736179202</v>
       </c>
       <c r="C12" s="4">
-        <v>3056.9459999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>2685.19005305272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
-        <v>500</v>
+        <v>12500</v>
       </c>
       <c r="B13" s="4">
-        <v>3020.69</v>
+        <v>2659.3201704624298</v>
       </c>
       <c r="C13" s="4">
-        <v>3041.0819999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>2665.6838978021101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
-        <v>1000</v>
+        <v>13750</v>
       </c>
       <c r="B14" s="4">
-        <v>3022.886</v>
+        <v>2655.0055489285101</v>
       </c>
       <c r="C14" s="4">
-        <v>3035.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>2661.4637059946499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="B15" s="4">
-        <v>3026.1486195945899</v>
-      </c>
-      <c r="C15" s="5">
-        <v>3033.5014479266601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2653.61358654892</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2660.10233327369</v>
+      </c>
+      <c r="D15">
+        <v>2762.8317147870298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
-        <v>2250</v>
+        <v>16250</v>
       </c>
       <c r="B16" s="4">
-        <v>3026.7596919995999</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3033.4401349672598</v>
+        <v>2654.6577020670002</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2661.0960755036799</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
-        <v>2500</v>
+        <v>17500</v>
       </c>
       <c r="B17" s="4">
-        <v>3027.33922705942</v>
-      </c>
-      <c r="C17" s="5">
-        <v>3033.4954035617998</v>
+        <v>2657.69860241058</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2664.0482480256801</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4">
-        <v>2750</v>
+        <v>20000</v>
       </c>
       <c r="B18" s="4">
-        <v>3027.89424050959</v>
-      </c>
-      <c r="C18" s="5">
-        <v>3033.5673149961199</v>
+        <v>2668.4684627052802</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2674.5084717698301</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4">
-        <v>3000</v>
+        <v>22500</v>
       </c>
       <c r="B19" s="4">
-        <v>3028.4309984415299</v>
-      </c>
-      <c r="C19" s="5">
-        <v>3033.70893773649</v>
+        <v>2683.8195690552102</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2689.8180215029502</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4">
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="B20" s="4">
-        <v>3031.6889999999999</v>
+        <v>2702.2291197183999</v>
       </c>
       <c r="C20" s="4">
-        <v>3035.0540000000001</v>
+        <v>2708.14635910483</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4">
-        <v>7500</v>
+        <v>100000</v>
       </c>
       <c r="B21" s="4">
-        <v>3034.3780000000002</v>
+        <v>3165.25720450371</v>
       </c>
       <c r="C21" s="4">
-        <v>3037.2939999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4">
-        <v>10000</v>
-      </c>
-      <c r="B22" s="4">
-        <v>3036.2489999999998</v>
-      </c>
-      <c r="C22" s="4">
-        <v>3039.2840000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4">
-        <v>50000</v>
-      </c>
-      <c r="B23" s="4">
-        <v>3044.3786</v>
-      </c>
-      <c r="C23" s="4">
-        <v>3046.884</v>
+        <v>3170.5677963431199</v>
       </c>
     </row>
   </sheetData>
@@ -1678,6 +1607,7 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1688,22 +1618,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1713,215 +1643,273 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>0</v>
       </c>
       <c r="B3" s="4">
-        <v>3025.21</v>
+        <v>3025.6371486635799</v>
       </c>
       <c r="C3" s="4">
-        <v>3101.17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>3040.1088096751801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3025.1789295295598</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3067.09072223779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="4">
-        <v>3024.15962077936</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3054.65295548633</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4">
+      <c r="B5" s="4">
+        <v>3023.8879239692501</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3052.06070007674</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4">
         <v>100</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>3016.1990488709298</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>3028.7253154241998</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4">
+    <row r="7" spans="1:4">
+      <c r="A7" s="4">
         <v>1000</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>2953.1959239918301</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>2960.4490434786699</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4">
-        <v>2000</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2893.8460942936399</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2900.6828937670498</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="B8" s="4">
-        <v>2794.4054303942999</v>
+        <v>2752.6938971337599</v>
       </c>
       <c r="C8" s="4">
-        <v>2800.5340608912202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>2758.3636996005398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
-        <v>8000</v>
+        <v>7500</v>
       </c>
       <c r="B9" s="4">
-        <v>2654.1603664709601</v>
+        <v>2668.1112975251399</v>
       </c>
       <c r="C9" s="4">
-        <v>2658.5967097054499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2672.74166088723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
-        <v>16000</v>
+        <v>10000</v>
       </c>
       <c r="B10" s="4">
-        <v>2526.44621010423</v>
+        <v>2606.8041008955202</v>
       </c>
       <c r="C10" s="4">
-        <v>2530.2591077406601</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>2610.7827800335099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
+        <v>12500</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2563.7920331788901</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2567.6591512618902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4">
+        <v>15000</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2534.8525465675898</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2538.73793270944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4">
+        <v>17500</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2516.6576203127001</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2520.32448975957</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4">
         <v>20000</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B14" s="4">
         <v>2506.4881668859398</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C14" s="4">
         <v>2509.8782304288302</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4">
-        <v>22000</v>
-      </c>
-      <c r="B12" s="4">
-        <v>2502.9837188041802</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2506.1765188539298</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4">
-        <v>24000</v>
-      </c>
-      <c r="B13" s="4">
-        <v>2502.7307192744802</v>
-      </c>
-      <c r="C13" s="4">
-        <v>2505.7119219208998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4">
-        <v>28000</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2509.3405617571698</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2511.85128985855</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
-        <v>32000</v>
+        <v>22500</v>
       </c>
       <c r="B15" s="4">
-        <v>2522.3347668854199</v>
+        <v>2502.64805833735</v>
       </c>
       <c r="C15" s="4">
-        <v>2524.8059217922901</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2505.7785906221402</v>
+      </c>
+      <c r="D15">
+        <v>2603.47044540148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
-        <v>64000</v>
+        <v>25000</v>
       </c>
       <c r="B16" s="4">
-        <v>2676.9150219215899</v>
+        <v>2503.5784100313799</v>
       </c>
       <c r="C16" s="4">
-        <v>2677.8755733368098</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3">
+        <v>2506.4759881461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2812.6307294770399</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2813.2605499669298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1938,20 +1926,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
@@ -2097,96 +2085,204 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3001.3894716713598</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3003.16200160587</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="A16" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2636.0388456547298</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2636.6051546178301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>20000</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2490.5757647813198</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2490.9906571699198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4">
+        <v>22500</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2479.1422512086301</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2479.5259110800998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4">
+        <v>25000</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2474.16247523325</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2474.47339852195</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2527.3180882524198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4">
+        <v>27500</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2474.3394389404498</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2474.7156888822001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="4">
+        <v>30000</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2478.7924672006502</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2479.1525559116699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4">
+        <v>35000</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2497.6289651862598</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2497.96493317565</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4">
+        <v>40000</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2524.68292928142</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2524.96828762106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2589.6423771848099</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2589.8805148217202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B25" s="4">
+        <v>2865.4961167035099</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2865.79294982687</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
New Figures Cool weighted output steez
</commit_message>
<xml_diff>
--- a/data/PartOne/Results/CrossValidation.xlsx
+++ b/data/PartOne/Results/CrossValidation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>lambda</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Gradient Descent Standardized lr = 0.1</t>
+  </si>
+  <si>
+    <t>Gradient Descent</t>
+  </si>
+  <si>
+    <t>Train Error</t>
   </si>
 </sst>
 </file>
@@ -96,7 +102,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,8 +192,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,8 +239,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -259,6 +288,16 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -303,6 +342,16 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -634,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -648,25 +697,25 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="9"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -1367,17 +1416,17 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D21" sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
@@ -1533,7 +1582,7 @@
         <v>2660.10233327369</v>
       </c>
       <c r="D15">
-        <v>2762.8317147870298</v>
+        <v>2761.5931339776598</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1618,27 +1667,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D17" sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="C1" s="9"/>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -1647,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -1658,7 +1710,7 @@
         <v>3040.1088096751801</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1669,7 +1721,7 @@
         <v>3067.09072223779</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -1680,7 +1732,7 @@
         <v>3052.06070007674</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>100</v>
       </c>
@@ -1691,7 +1743,7 @@
         <v>3028.7253154241998</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="4">
         <v>1000</v>
       </c>
@@ -1702,7 +1754,7 @@
         <v>2960.4490434786699</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
         <v>5000</v>
       </c>
@@ -1713,7 +1765,7 @@
         <v>2758.3636996005398</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="4">
         <v>7500</v>
       </c>
@@ -1724,7 +1776,7 @@
         <v>2672.74166088723</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
         <v>10000</v>
       </c>
@@ -1735,7 +1787,7 @@
         <v>2610.7827800335099</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <v>12500</v>
       </c>
@@ -1746,7 +1798,7 @@
         <v>2567.6591512618902</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
         <v>15000</v>
       </c>
@@ -1757,7 +1809,7 @@
         <v>2538.73793270944</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
         <v>17500</v>
       </c>
@@ -1768,7 +1820,7 @@
         <v>2520.32448975957</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
         <v>20000</v>
       </c>
@@ -1779,7 +1831,7 @@
         <v>2509.8782304288302</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="4">
         <v>22500</v>
       </c>
@@ -1790,10 +1842,10 @@
         <v>2505.7785906221402</v>
       </c>
       <c r="D15">
-        <v>2603.47044540148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>2607.0961787871502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>25000</v>
       </c>
@@ -1916,6 +1968,7 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1928,31 +1981,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D25" sqref="A2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -1963,7 +2019,7 @@
         <v>3040.1448029746298</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1974,7 +2030,7 @@
         <v>3031.4417756527</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>2.5</v>
       </c>
@@ -1985,7 +2041,7 @@
         <v>3029.0598462768899</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>3.75</v>
       </c>
@@ -1996,7 +2052,7 @@
         <v>3027.9896644933301</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -2007,7 +2063,7 @@
         <v>3027.3211312080598</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>5.625</v>
       </c>
@@ -2018,7 +2074,7 @@
         <v>3027.0903019472698</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>6.25</v>
       </c>
@@ -2029,7 +2085,7 @@
         <v>3026.9129466815398</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>7.5</v>
       </c>
@@ -2040,7 +2096,7 @@
         <v>3026.7882630526301</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
         <v>8.75</v>
       </c>
@@ -2051,7 +2107,7 @@
         <v>3026.7943327666999</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -2062,7 +2118,7 @@
         <v>3026.8143486607801</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
         <v>50</v>
       </c>
@@ -2073,7 +2129,7 @@
         <v>3028.9408412483299</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>100</v>
       </c>
@@ -2084,7 +2140,7 @@
         <v>3030.6767886459902</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
         <v>1000</v>
       </c>
@@ -2095,7 +2151,7 @@
         <v>3003.16200160587</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>10000</v>
       </c>
@@ -2139,7 +2195,7 @@
         <v>2474.47339852195</v>
       </c>
       <c r="D19" s="4">
-        <v>2527.3180882524198</v>
+        <v>2569.3249814902301</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2283,6 +2339,7 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>